<commit_message>
started on reg emp
</commit_message>
<xml_diff>
--- a/docs/Sprint5_Backlog.xlsx
+++ b/docs/Sprint5_Backlog.xlsx
@@ -69,9 +69,6 @@
     <t>As an Unregistered User I can view the Homepage</t>
   </si>
   <si>
-    <t>As an Unregistered User I can view the Register/Login</t>
-  </si>
-  <si>
     <t xml:space="preserve">As an Investor I can View my Companies </t>
   </si>
   <si>
@@ -121,6 +118,9 @@
   </si>
   <si>
     <t>As a Lawyer/Reviewer I can leave comments on a reserved Form</t>
+  </si>
+  <si>
+    <t>As an Unregistered User I can  Register/Login</t>
   </si>
 </sst>
 </file>
@@ -488,7 +488,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,7 +544,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="C3">
         <v>8</v>
@@ -564,7 +564,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4">
         <v>5</v>
@@ -584,7 +584,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5">
         <v>13</v>
@@ -604,7 +604,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6">
         <v>8</v>
@@ -624,7 +624,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7">
         <v>3</v>
@@ -644,7 +644,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C8">
         <v>8</v>
@@ -664,7 +664,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -684,7 +684,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C10">
         <v>5</v>
@@ -704,7 +704,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11">
         <v>5</v>
@@ -724,7 +724,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C12">
         <v>5</v>
@@ -744,7 +744,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C13">
         <v>3</v>
@@ -764,7 +764,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C14">
         <v>5</v>
@@ -784,7 +784,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C15">
         <v>5</v>
@@ -804,7 +804,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C16">
         <v>5</v>
@@ -824,7 +824,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C17" s="2">
         <v>5</v>
@@ -844,7 +844,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C18">
         <v>8</v>
@@ -864,7 +864,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C19">
         <v>5</v>
@@ -884,7 +884,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C20">
         <v>5</v>

</xml_diff>